<commit_message>
Gestione: aggiornati TODO e ore
</commit_message>
<xml_diff>
--- a/Assets/Dialogues/LaRiscrittora/Ore dedicate.xlsx
+++ b/Assets/Dialogues/LaRiscrittora/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Dialogues\LaRiscrittora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D89D6D-5294-4525-B576-EAFAF69D37EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FD29EB-2BF4-4C72-947A-304A43D23F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Data</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Accorpati i progetti</t>
+  </si>
+  <si>
+    <t>Funzioni di cambio luogo + background base</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -211,7 +214,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -492,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +585,7 @@
       </c>
       <c r="F4" s="7">
         <f>SUM(D:D)</f>
-        <v>0.90625</v>
+        <v>0.94791666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -695,8 +697,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="8"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>